<commit_message>
ajuste a documento existente
</commit_message>
<xml_diff>
--- a/NextLoad/Files/ajuste_entrada.xlsx
+++ b/NextLoad/Files/ajuste_entrada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\ac\developer\c#\NextLoad\NextLoad\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,9 +65,6 @@
     <t>Cost. Unit. (BSD)</t>
   </si>
   <si>
-    <t>US$</t>
-  </si>
-  <si>
     <t>Fec. Elaboracion</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>20240623018</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -467,9 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -514,10 +512,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -534,7 +532,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F2" s="5">
         <v>40</v>
@@ -543,7 +541,7 @@
         <v>4000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -569,7 +567,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F3" s="5">
         <v>40</v>
@@ -578,7 +576,7 @@
         <v>4000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -604,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5">
         <v>40</v>
@@ -613,7 +611,7 @@
         <v>4000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -639,7 +637,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5">
         <v>40</v>
@@ -648,7 +646,7 @@
         <v>4000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -674,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F6" s="5">
         <v>40</v>
@@ -683,7 +681,7 @@
         <v>4000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -700,7 +698,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -709,7 +707,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5">
         <v>40</v>
@@ -718,7 +716,7 @@
         <v>2000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -735,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -744,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5">
         <v>40</v>
@@ -753,7 +751,7 @@
         <v>2000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -770,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -779,7 +777,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5">
         <v>40</v>
@@ -788,7 +786,7 @@
         <v>2000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -805,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -814,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5">
         <v>40</v>
@@ -823,7 +821,7 @@
         <v>2000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -840,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -849,7 +847,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F11" s="5">
         <v>40</v>
@@ -858,7 +856,7 @@
         <v>2000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -875,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -884,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F12" s="5">
         <v>40</v>
@@ -893,7 +891,7 @@
         <v>2000</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -910,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -919,7 +917,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F13" s="5">
         <v>40</v>
@@ -928,7 +926,7 @@
         <v>2000</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -942,10 +940,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -954,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F14" s="5">
         <v>40</v>
@@ -963,7 +961,7 @@
         <v>3000</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14">
         <v>5</v>
@@ -977,10 +975,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -989,7 +987,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F15" s="5">
         <v>40</v>
@@ -998,7 +996,7 @@
         <v>3000</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15">
         <v>5</v>
@@ -1012,11 +1010,11 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
@@ -1024,7 +1022,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F16" s="5">
         <v>40</v>
@@ -1033,7 +1031,7 @@
         <v>1500</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1047,11 +1045,11 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F17" s="5">
         <v>40</v>
@@ -1068,7 +1066,7 @@
         <v>1500</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1082,11 +1080,11 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
@@ -1094,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F18" s="5">
         <v>40</v>
@@ -1103,7 +1101,7 @@
         <v>1500</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1117,11 +1115,11 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F19" s="5">
         <v>40</v>
@@ -1138,7 +1136,7 @@
         <v>1500</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I19">
         <v>2</v>

</xml_diff>